<commit_message>
Update to links to Dependency nodes.
</commit_message>
<xml_diff>
--- a/testing/pwtp_wa_anon_model.xlsx
+++ b/testing/pwtp_wa_anon_model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16440" tabRatio="788" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16440" tabRatio="788" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="system_meta" sheetId="17" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Tanks" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">component_connections!$A$1:$E$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">component_connections!$A$1:$E$107</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">component_list!$A$1:$I$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">excluded_components!#REF!</definedName>
     <definedName name="COMPONENT_LOCATION_CONF">OFFSET(VALIDATION_TABLES!$D$2,0,0,COUNTA(VALIDATION_TABLES!$D$2:$D$201),1)</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2859" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="403">
   <si>
     <t>component_type</t>
   </si>
@@ -4447,7 +4447,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5774,9 +5774,9 @@
   </sheetPr>
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5964,7 +5964,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="4">
-        <v>460</v>
+        <v>780</v>
       </c>
       <c r="I6" s="4">
         <v>895</v>
@@ -7969,11 +7969,11 @@
   <sheetPr>
     <tabColor rgb="FF66CCFF"/>
   </sheetPr>
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C78" sqref="C78:D81"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8290,7 +8290,7 @@
         <v>204</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C22" s="38">
         <v>1</v>
@@ -8303,8 +8303,8 @@
       <c r="A23" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>381</v>
+      <c r="B23" s="128" t="s">
+        <v>163</v>
       </c>
       <c r="C23" s="38">
         <v>1</v>
@@ -8318,7 +8318,7 @@
         <v>204</v>
       </c>
       <c r="B24" s="128" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C24" s="38">
         <v>1</v>
@@ -8328,25 +8328,28 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="125" t="s">
         <v>204</v>
       </c>
-      <c r="B25" s="128" t="s">
-        <v>173</v>
-      </c>
-      <c r="C25" s="38">
-        <v>1</v>
-      </c>
-      <c r="D25" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="125" t="s">
+        <v>400</v>
+      </c>
+      <c r="C25" s="126">
+        <v>1</v>
+      </c>
+      <c r="D25" s="127">
+        <v>1</v>
+      </c>
+      <c r="E25" s="65" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="125" t="s">
-        <v>204</v>
+        <v>400</v>
       </c>
       <c r="B26" s="125" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C26" s="126">
         <v>1</v>
@@ -8354,44 +8357,41 @@
       <c r="D26" s="127">
         <v>1</v>
       </c>
-      <c r="E26" s="65" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="125" t="s">
-        <v>400</v>
-      </c>
-      <c r="B27" s="125" t="s">
-        <v>395</v>
-      </c>
-      <c r="C27" s="126">
-        <v>1</v>
-      </c>
-      <c r="D27" s="127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="46" t="s">
+    </row>
+    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B27" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="C28" s="47">
-        <v>1</v>
-      </c>
-      <c r="D28" s="48">
+      <c r="C27" s="47">
+        <v>1</v>
+      </c>
+      <c r="D27" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" s="38">
+        <v>1</v>
+      </c>
+      <c r="D28" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>201</v>
+        <v>136</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C29" s="38">
         <v>1</v>
@@ -8402,10 +8402,10 @@
     </row>
     <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>135</v>
+        <v>392</v>
       </c>
       <c r="C30" s="38">
         <v>1</v>
@@ -8416,10 +8416,10 @@
     </row>
     <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B31" s="2" t="s">
         <v>392</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>138</v>
       </c>
       <c r="C31" s="38">
         <v>1</v>
@@ -8430,10 +8430,10 @@
     </row>
     <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="B32" s="32" t="s">
         <v>138</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>390</v>
       </c>
       <c r="C32" s="38">
         <v>1</v>
@@ -8444,10 +8444,10 @@
     </row>
     <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>138</v>
+        <v>376</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>390</v>
+        <v>194</v>
       </c>
       <c r="C33" s="38">
         <v>1</v>
@@ -8461,7 +8461,7 @@
         <v>376</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C34" s="38">
         <v>1</v>
@@ -8475,10 +8475,10 @@
         <v>376</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C35" s="38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" s="39">
         <v>1</v>
@@ -8489,7 +8489,7 @@
         <v>376</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C36" s="38">
         <v>2</v>
@@ -8503,7 +8503,7 @@
         <v>376</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C37" s="38">
         <v>2</v>
@@ -8516,8 +8516,8 @@
       <c r="A38" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B38" s="31" t="s">
-        <v>198</v>
+      <c r="B38" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C38" s="38">
         <v>2</v>
@@ -8527,14 +8527,14 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>376</v>
+      <c r="A39" s="31" t="s">
+        <v>194</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>199</v>
+        <v>220</v>
       </c>
       <c r="C39" s="38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="39">
         <v>1</v>
@@ -8542,7 +8542,7 @@
     </row>
     <row r="40" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>220</v>
@@ -8556,13 +8556,13 @@
     </row>
     <row r="41" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C41" s="38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D41" s="39">
         <v>1</v>
@@ -8570,7 +8570,7 @@
     </row>
     <row r="42" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>220</v>
@@ -8584,7 +8584,7 @@
     </row>
     <row r="43" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>220</v>
@@ -8597,8 +8597,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
-        <v>198</v>
+      <c r="A44" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>220</v>
@@ -8612,13 +8612,13 @@
     </row>
     <row r="45" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>199</v>
+        <v>377</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>220</v>
+        <v>164</v>
       </c>
       <c r="C45" s="38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" s="39">
         <v>1</v>
@@ -8629,49 +8629,49 @@
         <v>377</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" s="38">
+        <v>1</v>
+      </c>
+      <c r="D46" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="66" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C46" s="38">
-        <v>1</v>
-      </c>
-      <c r="D46" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C47" s="38">
-        <v>1</v>
-      </c>
-      <c r="D47" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="66" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="40">
+        <v>1</v>
+      </c>
+      <c r="D47" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C48" s="40">
-        <v>1</v>
-      </c>
-      <c r="D48" s="41">
+        <v>165</v>
+      </c>
+      <c r="C48" s="38">
+        <v>1</v>
+      </c>
+      <c r="D48" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>165</v>
+        <v>390</v>
       </c>
       <c r="C49" s="38">
         <v>1</v>
@@ -8681,22 +8681,25 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B50" s="2" t="s">
+      <c r="A50" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" s="22" t="s">
         <v>390</v>
       </c>
-      <c r="C50" s="38">
-        <v>1</v>
-      </c>
-      <c r="D50" s="39">
-        <v>1</v>
+      <c r="C50" s="42">
+        <v>1</v>
+      </c>
+      <c r="D50" s="43">
+        <v>1</v>
+      </c>
+      <c r="E50" s="65" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B51" s="22" t="s">
         <v>390</v>
@@ -8707,58 +8710,55 @@
       <c r="D51" s="43">
         <v>1</v>
       </c>
-      <c r="E51" s="65" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="B52" s="22" t="s">
+    </row>
+    <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="34" t="s">
         <v>390</v>
       </c>
-      <c r="C52" s="42">
-        <v>1</v>
-      </c>
-      <c r="D52" s="43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="34" t="s">
-        <v>390</v>
-      </c>
-      <c r="B53" s="34" t="s">
+      <c r="B52" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="44">
-        <v>1</v>
-      </c>
-      <c r="D53" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="46" t="s">
+      <c r="C52" s="44">
+        <v>1</v>
+      </c>
+      <c r="D52" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="B54" s="46" t="s">
+      <c r="B53" s="46" t="s">
         <v>391</v>
       </c>
-      <c r="C54" s="47">
-        <v>1</v>
-      </c>
-      <c r="D54" s="48">
+      <c r="C53" s="47">
+        <v>1</v>
+      </c>
+      <c r="D53" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C54" s="38">
+        <v>1</v>
+      </c>
+      <c r="D54" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C55" s="38">
         <v>1</v>
@@ -8769,10 +8769,10 @@
     </row>
     <row r="56" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>391</v>
+        <v>140</v>
       </c>
       <c r="C56" s="38">
         <v>1</v>
@@ -8783,10 +8783,10 @@
     </row>
     <row r="57" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>391</v>
+        <v>140</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>140</v>
+        <v>394</v>
       </c>
       <c r="C57" s="38">
         <v>1</v>
@@ -8794,13 +8794,16 @@
       <c r="D57" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="65" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>140</v>
+        <v>394</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="C58" s="38">
         <v>1</v>
@@ -8808,44 +8811,41 @@
       <c r="D58" s="39">
         <v>1</v>
       </c>
-      <c r="E58" s="65" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C59" s="38">
-        <v>1</v>
-      </c>
-      <c r="D59" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="46" t="s">
+    </row>
+    <row r="59" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="B60" s="46" t="s">
+      <c r="B59" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="C60" s="47">
-        <v>1</v>
-      </c>
-      <c r="D60" s="48">
+      <c r="C59" s="47">
+        <v>1</v>
+      </c>
+      <c r="D59" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C60" s="38">
+        <v>1</v>
+      </c>
+      <c r="D60" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>137</v>
+        <v>378</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>378</v>
+        <v>394</v>
       </c>
       <c r="C61" s="38">
         <v>1</v>
@@ -8856,10 +8856,10 @@
     </row>
     <row r="62" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="C62" s="38">
         <v>1</v>
@@ -8868,12 +8868,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>381</v>
+        <v>132</v>
       </c>
       <c r="C63" s="38">
         <v>1</v>
@@ -8882,31 +8882,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="B64" s="2" t="s">
+    <row r="64" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="C64" s="38">
-        <v>1</v>
-      </c>
-      <c r="D64" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="B65" s="46" t="s">
+      <c r="B64" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C65" s="47">
-        <v>1</v>
-      </c>
-      <c r="D65" s="48">
+      <c r="C64" s="47">
+        <v>1</v>
+      </c>
+      <c r="D64" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C65" s="38">
+        <v>1</v>
+      </c>
+      <c r="D65" s="39">
         <v>1</v>
       </c>
     </row>
@@ -8915,7 +8915,7 @@
         <v>133</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C66" s="38">
         <v>1</v>
@@ -8925,11 +8925,11 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>397</v>
+      <c r="A67" s="178" t="s">
+        <v>380</v>
+      </c>
+      <c r="B67" s="178" t="s">
+        <v>173</v>
       </c>
       <c r="C67" s="38">
         <v>1</v>
@@ -8943,7 +8943,7 @@
         <v>380</v>
       </c>
       <c r="B68" s="178" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C68" s="38">
         <v>1</v>
@@ -8957,7 +8957,7 @@
         <v>380</v>
       </c>
       <c r="B69" s="178" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="C69" s="38">
         <v>1</v>
@@ -8971,7 +8971,7 @@
         <v>380</v>
       </c>
       <c r="B70" s="178" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C70" s="38">
         <v>1</v>
@@ -8985,7 +8985,7 @@
         <v>380</v>
       </c>
       <c r="B71" s="178" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C71" s="38">
         <v>1</v>
@@ -8999,7 +8999,7 @@
         <v>380</v>
       </c>
       <c r="B72" s="178" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C72" s="38">
         <v>1</v>
@@ -9010,16 +9010,19 @@
     </row>
     <row r="73" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="178" t="s">
-        <v>380</v>
+        <v>173</v>
       </c>
       <c r="B73" s="178" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C73" s="38">
         <v>1</v>
       </c>
       <c r="D73" s="39">
         <v>1</v>
+      </c>
+      <c r="E73" s="54" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9027,30 +9030,30 @@
         <v>173</v>
       </c>
       <c r="B74" s="178" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C74" s="38">
         <v>1</v>
       </c>
       <c r="D74" s="39">
         <v>1</v>
-      </c>
-      <c r="E74" s="54" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="178" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B75" s="178" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C75" s="38">
         <v>1</v>
       </c>
       <c r="D75" s="39">
         <v>1</v>
+      </c>
+      <c r="E75" s="54" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9058,24 +9061,21 @@
         <v>163</v>
       </c>
       <c r="B76" s="178" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C76" s="38">
         <v>1</v>
       </c>
       <c r="D76" s="39">
         <v>1</v>
-      </c>
-      <c r="E76" s="54" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="178" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="B77" s="178" t="s">
-        <v>177</v>
+        <v>362</v>
       </c>
       <c r="C77" s="38">
         <v>1</v>
@@ -9086,7 +9086,7 @@
     </row>
     <row r="78" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="178" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B78" s="178" t="s">
         <v>362</v>
@@ -9100,7 +9100,7 @@
     </row>
     <row r="79" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="178" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B79" s="178" t="s">
         <v>362</v>
@@ -9114,7 +9114,7 @@
     </row>
     <row r="80" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="178" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B80" s="178" t="s">
         <v>362</v>
@@ -9127,11 +9127,11 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="178" t="s">
-        <v>177</v>
-      </c>
-      <c r="B81" s="178" t="s">
-        <v>362</v>
+      <c r="A81" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>396</v>
       </c>
       <c r="C81" s="38">
         <v>1</v>
@@ -9139,72 +9139,72 @@
       <c r="D81" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E81" s="54" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>398</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C82" s="38">
+        <v>1</v>
+      </c>
+      <c r="D82" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="B83" s="46" t="s">
+        <v>208</v>
+      </c>
+      <c r="C83" s="47">
+        <v>1</v>
+      </c>
+      <c r="D83" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="C82" s="38">
-        <v>1</v>
-      </c>
-      <c r="D82" s="39">
-        <v>1</v>
-      </c>
-      <c r="E82" s="54" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C83" s="38">
-        <v>1</v>
-      </c>
-      <c r="D83" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="46" t="s">
-        <v>203</v>
-      </c>
-      <c r="B84" s="46" t="s">
-        <v>208</v>
-      </c>
-      <c r="C84" s="47">
-        <v>1</v>
-      </c>
-      <c r="D84" s="48">
+      <c r="B84" s="177" t="s">
+        <v>360</v>
+      </c>
+      <c r="C84" s="38">
+        <v>1</v>
+      </c>
+      <c r="D84" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B85" s="177" t="s">
+        <v>361</v>
+      </c>
+      <c r="C85" s="38">
+        <v>1</v>
+      </c>
+      <c r="D85" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="177" t="s">
         <v>360</v>
       </c>
-      <c r="C85" s="38">
-        <v>1</v>
-      </c>
-      <c r="D85" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>397</v>
-      </c>
       <c r="B86" s="177" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C86" s="38">
         <v>1</v>
@@ -9215,7 +9215,7 @@
     </row>
     <row r="87" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="177" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B87" s="177" t="s">
         <v>362</v>
@@ -9229,10 +9229,10 @@
     </row>
     <row r="88" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="177" t="s">
-        <v>361</v>
-      </c>
-      <c r="B88" s="177" t="s">
         <v>362</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C88" s="38">
         <v>1</v>
@@ -9246,7 +9246,7 @@
         <v>362</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="C89" s="38">
         <v>1</v>
@@ -9260,7 +9260,7 @@
         <v>362</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="C90" s="38">
         <v>1</v>
@@ -9274,7 +9274,7 @@
         <v>362</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>70</v>
+        <v>153</v>
       </c>
       <c r="C91" s="38">
         <v>1</v>
@@ -9284,11 +9284,11 @@
       </c>
     </row>
     <row r="92" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="177" t="s">
-        <v>362</v>
+      <c r="A92" s="2" t="s">
+        <v>402</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="C92" s="38">
         <v>1</v>
@@ -9302,7 +9302,7 @@
         <v>402</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="C93" s="38">
         <v>1</v>
@@ -9316,7 +9316,7 @@
         <v>402</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="C94" s="38">
         <v>1</v>
@@ -9330,7 +9330,7 @@
         <v>402</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>70</v>
+        <v>153</v>
       </c>
       <c r="C95" s="38">
         <v>1</v>
@@ -9341,10 +9341,10 @@
     </row>
     <row r="96" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>402</v>
+        <v>208</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="C96" s="38">
         <v>1</v>
@@ -9358,7 +9358,7 @@
         <v>208</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="C97" s="38">
         <v>1</v>
@@ -9372,7 +9372,7 @@
         <v>208</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="C98" s="38">
         <v>1</v>
@@ -9386,7 +9386,7 @@
         <v>208</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>70</v>
+        <v>153</v>
       </c>
       <c r="C99" s="38">
         <v>1</v>
@@ -9397,10 +9397,10 @@
     </row>
     <row r="100" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>208</v>
+        <v>69</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C100" s="38">
         <v>1</v>
@@ -9411,7 +9411,7 @@
     </row>
     <row r="101" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>154</v>
@@ -9425,7 +9425,7 @@
     </row>
     <row r="102" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>154</v>
@@ -9439,7 +9439,7 @@
     </row>
     <row r="103" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>70</v>
+        <v>153</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>154</v>
@@ -9453,11 +9453,11 @@
     </row>
     <row r="104" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B104" s="2" t="s">
         <v>154</v>
       </c>
+      <c r="B104" s="129" t="s">
+        <v>399</v>
+      </c>
       <c r="C104" s="38">
         <v>1</v>
       </c>
@@ -9466,8 +9466,8 @@
       </c>
     </row>
     <row r="105" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>154</v>
+      <c r="A105" s="33" t="s">
+        <v>203</v>
       </c>
       <c r="B105" s="129" t="s">
         <v>399</v>
@@ -9480,55 +9480,44 @@
       </c>
     </row>
     <row r="106" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="B106" s="129" t="s">
+      <c r="A106" s="129" t="s">
         <v>399</v>
       </c>
+      <c r="B106" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="C106" s="38">
         <v>1</v>
       </c>
       <c r="D106" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="129" t="s">
-        <v>399</v>
-      </c>
-      <c r="B107" s="2" t="s">
+      <c r="E106" s="67" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="C107" s="38">
-        <v>1</v>
-      </c>
-      <c r="D107" s="39">
-        <v>1</v>
-      </c>
-      <c r="E107" s="67" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="B108" s="34" t="s">
+      <c r="B107" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="C108" s="44">
-        <v>1</v>
-      </c>
-      <c r="D108" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="68"/>
-      <c r="B109" s="68"/>
-      <c r="C109" s="69"/>
-      <c r="D109" s="70"/>
+      <c r="C107" s="44">
+        <v>1</v>
+      </c>
+      <c r="D107" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="68"/>
+      <c r="B108" s="68"/>
+      <c r="C108" s="69"/>
+      <c r="D108" s="70"/>
+    </row>
+    <row r="109" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C109" s="71"/>
     </row>
     <row r="110" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C110" s="71"/>
@@ -9692,9 +9681,7 @@
     <row r="163" spans="3:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C163" s="71"/>
     </row>
-    <row r="164" spans="3:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C164" s="71"/>
-    </row>
+    <row r="164" spans="3:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="165" spans="3:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="166" spans="3:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="167" spans="3:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9707,11 +9694,10 @@
     <row r="174" spans="3:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="175" spans="3:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="176" spans="3:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A109:B249">
-      <formula1>$A$2:$A$82</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A108:B248">
+      <formula1>$A$2:$A$81</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9729,7 +9715,7 @@
           <x14:formula1>
             <xm:f>component_list!$A$2:$A$71</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:B108</xm:sqref>
+          <xm:sqref>A2:B107</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>